<commit_message>
LC of capital doesn't need ipopt, fixing input script and regolding with 4 yr project
</commit_message>
<xml_diff>
--- a/tests/integration_tests/mechanics/levelized_cost/analytic.xlsx
+++ b/tests/integration_tests/mechanics/levelized_cost/analytic.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sotogj\projects\HERON\tests\integration_tests\mechanics\levelized_cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F06A6EF-8BFF-40C5-9D64-BBCEF5A7B5AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31419368-1C7C-47F9-8E63-C6E9E4774307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="3" xr2:uid="{C5D1EC3D-253D-D049-ACFA-71EC9987361D}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="465" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="467" uniqueCount="78">
   <si>
     <t>CASE VARIABLES</t>
   </si>
@@ -262,10 +262,16 @@
     <t>Difference: we are multiplying price by Signal</t>
   </si>
   <si>
-    <t>Percentage</t>
+    <t>(LIFETIME --&gt;)</t>
   </si>
   <si>
-    <t>(LIFETIME --&gt;)</t>
+    <t>POSITIVE CF</t>
+  </si>
+  <si>
+    <t>NEGATIVE CF (taxed)</t>
+  </si>
+  <si>
+    <t>Amortization Percent</t>
   </si>
 </sst>
 </file>
@@ -276,7 +282,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -309,6 +315,14 @@
       <b/>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -568,7 +582,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="47">
+  <cellXfs count="48">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -590,9 +604,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -601,9 +612,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -618,6 +626,33 @@
     <xf numFmtId="164" fontId="2" fillId="8" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -636,36 +671,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -984,8 +995,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EE30361-7298-9048-9EE6-65784B82D934}">
   <dimension ref="A1:AF84"/>
   <sheetViews>
-    <sheetView topLeftCell="A39" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35:V37"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q49" sqref="Q49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1042,7 +1053,7 @@
       <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="24">
         <v>0.08</v>
       </c>
     </row>
@@ -1058,7 +1069,7 @@
       <c r="A9" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="24">
         <v>0.25</v>
       </c>
     </row>
@@ -2279,70 +2290,70 @@
     </row>
     <row r="34" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="37" t="s">
+      <c r="D35" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="44" t="s">
+      <c r="E35" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="44" t="s">
+      <c r="F35" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="44" t="s">
+      <c r="G35" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="H35" s="44" t="s">
+      <c r="H35" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I35" s="44" t="s">
+      <c r="I35" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="J35" s="44" t="s">
+      <c r="J35" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="K35" s="44" t="s">
+      <c r="K35" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="44" t="s">
+      <c r="L35" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="M35" s="44" t="s">
+      <c r="M35" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="N35" s="44" t="s">
+      <c r="N35" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="O35" s="44" t="s">
+      <c r="O35" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="P35" s="44" t="s">
+      <c r="P35" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q35" s="44" t="s">
+      <c r="Q35" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="R35" s="44" t="s">
+      <c r="R35" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="S35" s="44" t="s">
+      <c r="S35" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="T35" s="44" t="s">
+      <c r="T35" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="U35" s="44" t="s">
+      <c r="U35" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="V35" s="44" t="s">
+      <c r="V35" s="35" t="s">
         <v>25</v>
       </c>
       <c r="W35" s="14"/>
@@ -2357,76 +2368,76 @@
       <c r="AF35" s="14"/>
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="38">
+      <c r="A36" s="38"/>
+      <c r="B36" s="30">
         <f>$B$42*($C$15/$B$43)^$B$44</f>
         <v>-1000</v>
       </c>
-      <c r="C36" s="39">
+      <c r="C36" s="17">
         <f>$X$29</f>
         <v>560.76919999999996</v>
       </c>
-      <c r="D36" s="40">
-        <f t="shared" ref="D36:U36" si="10">$X$29</f>
+      <c r="D36" s="31">
+        <f t="shared" ref="D36" si="10">$X$29</f>
         <v>560.76919999999996</v>
       </c>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="45"/>
-      <c r="R36" s="45"/>
-      <c r="S36" s="45"/>
-      <c r="T36" s="45"/>
-      <c r="U36" s="45"/>
-      <c r="V36" s="45"/>
-      <c r="W36" s="25"/>
-      <c r="X36" s="25"/>
-      <c r="Y36" s="25"/>
-      <c r="Z36" s="25"/>
-      <c r="AA36" s="25"/>
-      <c r="AB36" s="25"/>
-      <c r="AC36" s="25"/>
-      <c r="AD36" s="25"/>
-      <c r="AE36" s="25"/>
-      <c r="AF36" s="25"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="36"/>
+      <c r="O36" s="36"/>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="36"/>
+      <c r="R36" s="36"/>
+      <c r="S36" s="36"/>
+      <c r="T36" s="36"/>
+      <c r="U36" s="36"/>
+      <c r="V36" s="36"/>
+      <c r="W36" s="23"/>
+      <c r="X36" s="23"/>
+      <c r="Y36" s="23"/>
+      <c r="Z36" s="23"/>
+      <c r="AA36" s="23"/>
+      <c r="AB36" s="23"/>
+      <c r="AC36" s="23"/>
+      <c r="AD36" s="23"/>
+      <c r="AE36" s="23"/>
+      <c r="AF36" s="23"/>
     </row>
     <row r="37" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="41">
+      <c r="B37" s="32">
         <f>NPV($B$7,C36:AF36)+$B$36</f>
         <v>-5.4869684731784218E-5</v>
       </c>
-      <c r="C37" s="42"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="46"/>
-      <c r="K37" s="46"/>
-      <c r="L37" s="46"/>
-      <c r="M37" s="46"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="46"/>
-      <c r="P37" s="46"/>
-      <c r="Q37" s="46"/>
-      <c r="R37" s="46"/>
-      <c r="S37" s="46"/>
-      <c r="T37" s="46"/>
-      <c r="U37" s="46"/>
-      <c r="V37" s="46"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37"/>
+      <c r="Q37" s="37"/>
+      <c r="R37" s="37"/>
+      <c r="S37" s="37"/>
+      <c r="T37" s="37"/>
+      <c r="U37" s="37"/>
+      <c r="V37" s="37"/>
     </row>
     <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -2434,325 +2445,325 @@
       </c>
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="31"/>
+      <c r="B41" s="40"/>
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="21">
+      <c r="B42" s="20">
         <v>-1000</v>
       </c>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="20">
+      <c r="B43" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="20">
+      <c r="B44" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="20">
+      <c r="B45" s="19">
         <f>B2</f>
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="20" t="b">
+      <c r="B48" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="20" t="b">
+      <c r="B50" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="20">
+      <c r="B51" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B53" s="33"/>
+      <c r="B53" s="42"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="24">
+      <c r="B54" s="22">
         <v>-100</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="20">
+      <c r="B55" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="20">
+      <c r="B56" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B57" s="20">
+      <c r="B57" s="19">
         <f>B2</f>
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="19" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B60" s="20" t="b">
+      <c r="B60" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
+      <c r="A62" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B62" s="20" t="b">
+      <c r="B62" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="34" t="s">
+      <c r="A64" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B64" s="34"/>
+      <c r="B64" s="43"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="23" t="s">
+      <c r="A65" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="24">
+      <c r="B65" s="22">
         <v>-1</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B66" s="20">
+      <c r="B66" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B67" s="20">
+      <c r="B67" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B68" s="20">
+      <c r="B68" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
+      <c r="A69" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="19" t="s">
+      <c r="A70" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B70" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="19" t="s">
+      <c r="A71" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B71" s="20" t="b">
+      <c r="B71" s="19" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="19" t="s">
+      <c r="A73" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B73" s="20" t="b">
+      <c r="B73" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="32" t="s">
+      <c r="A75" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B75" s="33"/>
+      <c r="B75" s="42"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="27" t="s">
+      <c r="A76" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B76" s="28">
+      <c r="B76" s="26">
         <f>-32.2152</f>
         <v>-32.215200000000003</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B77" s="20" t="s">
+      <c r="B77" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="19" t="s">
+      <c r="A78" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B78" s="20">
+      <c r="B78" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B79" s="20">
+      <c r="B79" s="19">
         <v>-1</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
+      <c r="A80" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B80" s="20" t="s">
+      <c r="B80" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="19" t="s">
+      <c r="A81" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B81" s="20" t="s">
+      <c r="B81" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
+      <c r="A82" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B82" s="20" t="b">
+      <c r="B82" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="19" t="s">
+      <c r="A83" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B83" s="20" t="s">
+      <c r="B83" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="19" t="s">
+      <c r="A84" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B84" s="20" t="b">
+      <c r="B84" s="19" t="b">
         <v>0</v>
       </c>
     </row>
@@ -2832,7 +2843,7 @@
       <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="24">
         <v>0.08</v>
       </c>
     </row>
@@ -2848,7 +2859,7 @@
       <c r="A9" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="24">
         <v>0.25</v>
       </c>
     </row>
@@ -4069,70 +4080,70 @@
     </row>
     <row r="34" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="37" t="s">
+      <c r="D35" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="44" t="s">
+      <c r="E35" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="44" t="s">
+      <c r="F35" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="44" t="s">
+      <c r="G35" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="H35" s="44" t="s">
+      <c r="H35" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I35" s="44" t="s">
+      <c r="I35" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="J35" s="44" t="s">
+      <c r="J35" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="K35" s="44" t="s">
+      <c r="K35" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="44" t="s">
+      <c r="L35" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="M35" s="44" t="s">
+      <c r="M35" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="N35" s="44" t="s">
+      <c r="N35" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="O35" s="44" t="s">
+      <c r="O35" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="P35" s="44" t="s">
+      <c r="P35" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q35" s="44" t="s">
+      <c r="Q35" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="R35" s="44" t="s">
+      <c r="R35" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="S35" s="44" t="s">
+      <c r="S35" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="T35" s="44" t="s">
+      <c r="T35" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="U35" s="44" t="s">
+      <c r="U35" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="V35" s="44" t="s">
+      <c r="V35" s="35" t="s">
         <v>25</v>
       </c>
       <c r="W35" s="14"/>
@@ -4147,76 +4158,76 @@
       <c r="AF35" s="14"/>
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="38">
+      <c r="A36" s="38"/>
+      <c r="B36" s="30">
         <f>$B$42*($C$15/$B$43)^$B$44</f>
         <v>-1000</v>
       </c>
-      <c r="C36" s="39">
+      <c r="C36" s="17">
         <f>$X$29</f>
         <v>560.76921800153798</v>
       </c>
-      <c r="D36" s="40">
-        <f t="shared" ref="D36:U36" si="10">$X$29</f>
+      <c r="D36" s="31">
+        <f t="shared" ref="D36" si="10">$X$29</f>
         <v>560.76921800153798</v>
       </c>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="45"/>
-      <c r="R36" s="45"/>
-      <c r="S36" s="45"/>
-      <c r="T36" s="45"/>
-      <c r="U36" s="45"/>
-      <c r="V36" s="45"/>
-      <c r="W36" s="25"/>
-      <c r="X36" s="25"/>
-      <c r="Y36" s="25"/>
-      <c r="Z36" s="25"/>
-      <c r="AA36" s="25"/>
-      <c r="AB36" s="25"/>
-      <c r="AC36" s="25"/>
-      <c r="AD36" s="25"/>
-      <c r="AE36" s="25"/>
-      <c r="AF36" s="25"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="36"/>
+      <c r="O36" s="36"/>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="36"/>
+      <c r="R36" s="36"/>
+      <c r="S36" s="36"/>
+      <c r="T36" s="36"/>
+      <c r="U36" s="36"/>
+      <c r="V36" s="36"/>
+      <c r="W36" s="23"/>
+      <c r="X36" s="23"/>
+      <c r="Y36" s="23"/>
+      <c r="Z36" s="23"/>
+      <c r="AA36" s="23"/>
+      <c r="AB36" s="23"/>
+      <c r="AC36" s="23"/>
+      <c r="AD36" s="23"/>
+      <c r="AE36" s="23"/>
+      <c r="AF36" s="23"/>
     </row>
     <row r="37" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="41">
+      <c r="B37" s="32">
         <f>NPV($B$7,C36:AF36)+$B$36</f>
         <v>-2.2768176563658926E-5</v>
       </c>
-      <c r="C37" s="42"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="46"/>
-      <c r="K37" s="46"/>
-      <c r="L37" s="46"/>
-      <c r="M37" s="46"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="46"/>
-      <c r="P37" s="46"/>
-      <c r="Q37" s="46"/>
-      <c r="R37" s="46"/>
-      <c r="S37" s="46"/>
-      <c r="T37" s="46"/>
-      <c r="U37" s="46"/>
-      <c r="V37" s="46"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37"/>
+      <c r="Q37" s="37"/>
+      <c r="R37" s="37"/>
+      <c r="S37" s="37"/>
+      <c r="T37" s="37"/>
+      <c r="U37" s="37"/>
+      <c r="V37" s="37"/>
     </row>
     <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -4224,269 +4235,269 @@
       </c>
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="31"/>
+      <c r="B41" s="40"/>
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="21">
+      <c r="B42" s="20">
         <v>-1000</v>
       </c>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="20">
+      <c r="B43" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="20">
+      <c r="B44" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="20">
+      <c r="B45" s="19">
         <f>B2</f>
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="20" t="b">
+      <c r="B48" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="20" t="b">
+      <c r="B50" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="20">
+      <c r="B51" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B53" s="33"/>
+      <c r="B53" s="42"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="24">
+      <c r="B54" s="22">
         <v>-100</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="20">
+      <c r="B55" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="20">
+      <c r="B56" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B57" s="20">
+      <c r="B57" s="19">
         <f>B2</f>
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="19" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B60" s="20" t="b">
+      <c r="B60" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
+      <c r="A62" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B62" s="20" t="b">
+      <c r="B62" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="34" t="s">
+      <c r="A64" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B64" s="34"/>
+      <c r="B64" s="43"/>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A65" s="23" t="s">
+      <c r="A65" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="24">
+      <c r="B65" s="22">
         <v>-1</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B66" s="20">
+      <c r="B66" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B67" s="20">
+      <c r="B67" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B68" s="20">
+      <c r="B68" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
+      <c r="A69" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A70" s="19" t="s">
+      <c r="A70" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B70" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A71" s="19" t="s">
+      <c r="A71" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B71" s="20" t="b">
+      <c r="B71" s="19" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A73" s="19" t="s">
+      <c r="A73" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B73" s="20" t="b">
+      <c r="B73" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="32" t="s">
+      <c r="A75" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B75" s="33"/>
+      <c r="B75" s="42"/>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A76" s="27" t="s">
+      <c r="A76" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B76" s="28">
+      <c r="B76" s="26">
         <f>-58.9855</f>
         <v>-58.985500000000002</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B77" s="20" t="s">
+      <c r="B77" s="19" t="s">
         <v>43</v>
       </c>
       <c r="D77" s="5" t="s">
@@ -4497,58 +4508,58 @@
       <c r="G77" s="5"/>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A78" s="19" t="s">
+      <c r="A78" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B78" s="20">
+      <c r="B78" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B79" s="20">
+      <c r="B79" s="19">
         <v>-1</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
+      <c r="A80" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B80" s="20" t="s">
+      <c r="B80" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="19" t="s">
+      <c r="A81" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B81" s="20" t="s">
+      <c r="B81" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
+      <c r="A82" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B82" s="20" t="b">
+      <c r="B82" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="19" t="s">
+      <c r="A83" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B83" s="20" t="s">
+      <c r="B83" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="19" t="s">
+      <c r="A84" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B84" s="20" t="b">
+      <c r="B84" s="19" t="b">
         <v>0</v>
       </c>
     </row>
@@ -4568,8 +4579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B1D02177-EA88-4616-9679-3E3345E3E1FB}">
   <dimension ref="A1:AF84"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G62" sqref="G62"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35:V37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -4626,7 +4637,7 @@
       <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="24">
         <v>0.08</v>
       </c>
     </row>
@@ -4642,7 +4653,7 @@
       <c r="A9" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="24">
         <v>0.25</v>
       </c>
     </row>
@@ -5863,70 +5874,70 @@
     </row>
     <row r="34" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="35" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="B35" s="35" t="s">
+      <c r="B35" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C35" s="36" t="s">
+      <c r="C35" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D35" s="37" t="s">
+      <c r="D35" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="E35" s="44" t="s">
+      <c r="E35" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="F35" s="44" t="s">
+      <c r="F35" s="35" t="s">
         <v>9</v>
       </c>
-      <c r="G35" s="44" t="s">
+      <c r="G35" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="H35" s="44" t="s">
+      <c r="H35" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I35" s="44" t="s">
+      <c r="I35" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="J35" s="44" t="s">
+      <c r="J35" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="K35" s="44" t="s">
+      <c r="K35" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="L35" s="44" t="s">
+      <c r="L35" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="M35" s="44" t="s">
+      <c r="M35" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="N35" s="44" t="s">
+      <c r="N35" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="O35" s="44" t="s">
+      <c r="O35" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="P35" s="44" t="s">
+      <c r="P35" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q35" s="44" t="s">
+      <c r="Q35" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="R35" s="44" t="s">
+      <c r="R35" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="S35" s="44" t="s">
+      <c r="S35" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="T35" s="44" t="s">
+      <c r="T35" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="U35" s="44" t="s">
+      <c r="U35" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="V35" s="44" t="s">
+      <c r="V35" s="35" t="s">
         <v>25</v>
       </c>
       <c r="W35" s="14"/>
@@ -5941,76 +5952,76 @@
       <c r="AF35" s="14"/>
     </row>
     <row r="36" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A36" s="29"/>
-      <c r="B36" s="38">
+      <c r="A36" s="38"/>
+      <c r="B36" s="30">
         <f>$B$42*($C$15/$B$43)^$B$44</f>
         <v>-1000</v>
       </c>
-      <c r="C36" s="39">
+      <c r="C36" s="17">
         <f>$X$29</f>
         <v>560.76867499999992</v>
       </c>
-      <c r="D36" s="40">
-        <f t="shared" ref="D36:U36" si="10">$X$29</f>
+      <c r="D36" s="31">
+        <f t="shared" ref="D36" si="10">$X$29</f>
         <v>560.76867499999992</v>
       </c>
-      <c r="E36" s="45"/>
-      <c r="F36" s="45"/>
-      <c r="G36" s="45"/>
-      <c r="H36" s="45"/>
-      <c r="I36" s="45"/>
-      <c r="J36" s="45"/>
-      <c r="K36" s="45"/>
-      <c r="L36" s="45"/>
-      <c r="M36" s="45"/>
-      <c r="N36" s="45"/>
-      <c r="O36" s="45"/>
-      <c r="P36" s="45"/>
-      <c r="Q36" s="45"/>
-      <c r="R36" s="45"/>
-      <c r="S36" s="45"/>
-      <c r="T36" s="45"/>
-      <c r="U36" s="45"/>
-      <c r="V36" s="45"/>
-      <c r="W36" s="25"/>
-      <c r="X36" s="25"/>
-      <c r="Y36" s="25"/>
-      <c r="Z36" s="25"/>
-      <c r="AA36" s="25"/>
-      <c r="AB36" s="25"/>
-      <c r="AC36" s="25"/>
-      <c r="AD36" s="25"/>
-      <c r="AE36" s="25"/>
-      <c r="AF36" s="25"/>
+      <c r="E36" s="36"/>
+      <c r="F36" s="36"/>
+      <c r="G36" s="36"/>
+      <c r="H36" s="36"/>
+      <c r="I36" s="36"/>
+      <c r="J36" s="36"/>
+      <c r="K36" s="36"/>
+      <c r="L36" s="36"/>
+      <c r="M36" s="36"/>
+      <c r="N36" s="36"/>
+      <c r="O36" s="36"/>
+      <c r="P36" s="36"/>
+      <c r="Q36" s="36"/>
+      <c r="R36" s="36"/>
+      <c r="S36" s="36"/>
+      <c r="T36" s="36"/>
+      <c r="U36" s="36"/>
+      <c r="V36" s="36"/>
+      <c r="W36" s="23"/>
+      <c r="X36" s="23"/>
+      <c r="Y36" s="23"/>
+      <c r="Z36" s="23"/>
+      <c r="AA36" s="23"/>
+      <c r="AB36" s="23"/>
+      <c r="AC36" s="23"/>
+      <c r="AD36" s="23"/>
+      <c r="AE36" s="23"/>
+      <c r="AF36" s="23"/>
     </row>
     <row r="37" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="41">
+      <c r="B37" s="32">
         <f>NPV($B$7,C36:AF36)+$B$36</f>
         <v>-9.9108367658118368E-4</v>
       </c>
-      <c r="C37" s="42"/>
-      <c r="D37" s="43"/>
-      <c r="E37" s="46"/>
-      <c r="F37" s="46"/>
-      <c r="G37" s="46"/>
-      <c r="H37" s="46"/>
-      <c r="I37" s="46"/>
-      <c r="J37" s="46"/>
-      <c r="K37" s="46"/>
-      <c r="L37" s="46"/>
-      <c r="M37" s="46"/>
-      <c r="N37" s="46"/>
-      <c r="O37" s="46"/>
-      <c r="P37" s="46"/>
-      <c r="Q37" s="46"/>
-      <c r="R37" s="46"/>
-      <c r="S37" s="46"/>
-      <c r="T37" s="46"/>
-      <c r="U37" s="46"/>
-      <c r="V37" s="46"/>
+      <c r="C37" s="33"/>
+      <c r="D37" s="34"/>
+      <c r="E37" s="37"/>
+      <c r="F37" s="37"/>
+      <c r="G37" s="37"/>
+      <c r="H37" s="37"/>
+      <c r="I37" s="37"/>
+      <c r="J37" s="37"/>
+      <c r="K37" s="37"/>
+      <c r="L37" s="37"/>
+      <c r="M37" s="37"/>
+      <c r="N37" s="37"/>
+      <c r="O37" s="37"/>
+      <c r="P37" s="37"/>
+      <c r="Q37" s="37"/>
+      <c r="R37" s="37"/>
+      <c r="S37" s="37"/>
+      <c r="T37" s="37"/>
+      <c r="U37" s="37"/>
+      <c r="V37" s="37"/>
     </row>
     <row r="40" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
@@ -6018,324 +6029,324 @@
       </c>
     </row>
     <row r="41" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A41" s="30" t="s">
+      <c r="A41" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B41" s="31"/>
+      <c r="B41" s="40"/>
     </row>
     <row r="42" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A42" s="19" t="s">
+      <c r="A42" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B42" s="21">
+      <c r="B42" s="20">
         <v>-1000</v>
       </c>
     </row>
     <row r="43" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A43" s="19" t="s">
+      <c r="A43" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B43" s="20">
+      <c r="B43" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="A44" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B44" s="20">
+      <c r="B44" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="45" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="A45" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B45" s="20">
+      <c r="B45" s="19">
         <f>B2</f>
         <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="A46" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B46" s="20" t="s">
+      <c r="B46" s="19" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+      <c r="A47" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
+      <c r="A48" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B48" s="20" t="b">
+      <c r="B48" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
+      <c r="A49" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="A50" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B50" s="20" t="b">
+      <c r="B50" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+      <c r="A51" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B51" s="20">
+      <c r="B51" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="53" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="32" t="s">
+      <c r="A53" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B53" s="33"/>
+      <c r="B53" s="42"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="23" t="s">
+      <c r="A54" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B54" s="24">
+      <c r="B54" s="22">
         <v>-100</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="19" t="s">
+      <c r="A55" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B55" s="20">
+      <c r="B55" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
+      <c r="A56" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B56" s="20">
+      <c r="B56" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="s">
+      <c r="A57" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B57" s="20">
+      <c r="B57" s="19">
         <f>B2</f>
         <v>1</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
+      <c r="A58" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B58" s="20" t="s">
+      <c r="B58" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="s">
+      <c r="A59" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B59" s="19" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="s">
+      <c r="A60" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B60" s="20" t="b">
+      <c r="B60" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+      <c r="A61" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B61" s="20" t="s">
+      <c r="B61" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
+      <c r="A62" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B62" s="20" t="b">
+      <c r="B62" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="64" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="34" t="s">
+      <c r="A64" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B64" s="34"/>
+      <c r="B64" s="43"/>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A65" s="27" t="s">
+      <c r="A65" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B65" s="28">
+      <c r="B65" s="26">
         <v>-24.713100000000001</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="19" t="s">
+      <c r="A66" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B66" s="20">
+      <c r="B66" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="19" t="s">
+      <c r="A67" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B67" s="20">
+      <c r="B67" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
+      <c r="A68" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B68" s="20">
+      <c r="B68" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
+      <c r="A69" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B69" s="20" t="s">
+      <c r="B69" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="19" t="s">
+      <c r="A70" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B70" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="19" t="s">
+      <c r="A71" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B71" s="20" t="b">
+      <c r="B71" s="19" t="b">
         <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="19" t="s">
+      <c r="A72" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B72" s="20" t="s">
+      <c r="B72" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="19" t="s">
+      <c r="A73" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B73" s="20" t="b">
+      <c r="B73" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="32" t="s">
+      <c r="A75" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B75" s="33"/>
+      <c r="B75" s="42"/>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A76" s="19" t="s">
+      <c r="A76" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B76" s="20">
+      <c r="B76" s="19">
         <v>-50</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="19" t="s">
+      <c r="A77" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B77" s="20" t="s">
+      <c r="B77" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="19" t="s">
+      <c r="A78" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B78" s="20">
+      <c r="B78" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="19" t="s">
+      <c r="A79" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B79" s="20">
+      <c r="B79" s="19">
         <v>-1</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
+      <c r="A80" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B80" s="20" t="s">
+      <c r="B80" s="19" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="19" t="s">
+      <c r="A81" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B81" s="20" t="s">
+      <c r="B81" s="19" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
+      <c r="A82" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B82" s="20" t="b">
+      <c r="B82" s="19" t="b">
         <v>0</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="19" t="s">
+      <c r="A83" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B83" s="20" t="s">
+      <c r="B83" s="19" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="19" t="s">
+      <c r="A84" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B84" s="20" t="b">
+      <c r="B84" s="19" t="b">
         <v>0</v>
       </c>
     </row>
@@ -6353,16 +6364,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{580E6340-367E-40D2-98E8-6185962A3596}">
-  <dimension ref="A1:AF85"/>
+  <dimension ref="A1:AF86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="L53" sqref="L53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.125" customWidth="1"/>
+    <col min="2" max="2" width="21" customWidth="1"/>
     <col min="3" max="3" width="12.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6413,9 +6424,10 @@
       <c r="A7" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="26">
+      <c r="B7" s="24">
         <v>0.08</v>
       </c>
+      <c r="C7" s="47"/>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
@@ -6429,7 +6441,7 @@
       <c r="A9" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B9" s="26">
+      <c r="B9" s="24">
         <v>0.25</v>
       </c>
     </row>
@@ -6739,7 +6751,7 @@
         <v>46</v>
       </c>
       <c r="C17" s="6">
-        <f t="shared" ref="C17:W17" si="1">C16*(C15/$B$44)^$B$45</f>
+        <f t="shared" ref="C17:W17" si="1">C16*(C15/$B$45)^$B$46</f>
         <v>0</v>
       </c>
       <c r="D17" s="9">
@@ -6828,7 +6840,7 @@
         <v>49</v>
       </c>
       <c r="C18" s="8">
-        <f>$B$55</f>
+        <f>$B$56</f>
         <v>-100</v>
       </c>
       <c r="D18" s="16">
@@ -6897,7 +6909,7 @@
         <v>50</v>
       </c>
       <c r="C19" s="6">
-        <f>C18*(C15/$B$56)^$B$57</f>
+        <f>C18*(C15/$B$57)^$B$58</f>
         <v>-100</v>
       </c>
       <c r="D19" s="9">
@@ -6986,87 +6998,87 @@
         <v>47</v>
       </c>
       <c r="C20" s="8">
-        <f t="shared" ref="C20:W20" si="3">$B$66</f>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="D20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="E20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="F20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="G20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="H20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="I20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="J20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="K20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="L20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="M20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="N20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="O20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="P20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="Q20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="R20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="S20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="T20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="U20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="V20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
       <c r="W20" s="16">
-        <f t="shared" si="3"/>
+        <f>$B$67</f>
         <v>-1</v>
       </c>
     </row>
@@ -7079,83 +7091,83 @@
         <v>-0.75</v>
       </c>
       <c r="D21" s="13">
-        <f t="shared" ref="D21:W21" si="4">(D20*(D15/1)^1)*(1-$B$9)</f>
+        <f t="shared" ref="D21:W21" si="3">(D20*(D15/1)^1)*(1-$B$9)</f>
         <v>-0.75</v>
       </c>
       <c r="E21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="F21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="G21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="H21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="I21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="J21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="K21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="L21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="M21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="N21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="O21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="P21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="Q21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="R21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="S21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="T21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="U21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="V21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="W21" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="3"/>
         <v>-0.75</v>
       </c>
       <c r="X21" s="14" t="s">
@@ -7171,83 +7183,83 @@
         <v>-100.75</v>
       </c>
       <c r="D22" s="11">
-        <f t="shared" ref="D22:W22" si="5">D21+D19+D17</f>
+        <f t="shared" ref="D22:W22" si="4">D21+D19+D17</f>
         <v>-0.75</v>
       </c>
       <c r="E22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="F22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="G22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="H22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="I22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="J22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="K22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="L22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="M22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="N22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="O22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="P22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="Q22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="R22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="S22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="T22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="U22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="V22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="W22" s="11">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>-0.75</v>
       </c>
       <c r="X22" s="15">
@@ -7267,83 +7279,83 @@
         <v>-1</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" ref="D24:W24" si="6">-$B$2</f>
+        <f t="shared" ref="D24:W24" si="5">-$B$2</f>
         <v>-1</v>
       </c>
       <c r="E24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="F24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="G24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="H24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="I24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="J24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="K24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="L24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="M24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="N24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="O24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="P24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="Q24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="R24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="S24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="T24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="U24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="V24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
       <c r="W24" s="3">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>-1</v>
       </c>
     </row>
@@ -7352,87 +7364,87 @@
         <v>53</v>
       </c>
       <c r="C25" s="16">
-        <f>$B$77</f>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="D25" s="16">
-        <f t="shared" ref="D25:W25" si="7">$B$77</f>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="E25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="F25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="G25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="H25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="I25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="J25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="K25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="L25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="M25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="N25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="O25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="P25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="Q25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="R25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="S25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="T25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="U25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="V25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="W25" s="16">
-        <f t="shared" si="7"/>
+        <f>$B$78</f>
         <v>-50</v>
       </c>
       <c r="X25" s="14" t="s">
@@ -7448,83 +7460,83 @@
         <v>50</v>
       </c>
       <c r="D26" s="9">
-        <f t="shared" ref="D26:W26" si="8">D25*(D24/1)^1</f>
+        <f t="shared" ref="D26:W26" si="6">D25*(D24/1)^1</f>
         <v>50</v>
       </c>
       <c r="E26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="F26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="G26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="H26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="I26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="J26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="K26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="L26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="M26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="N26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="O26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="P26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="Q26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="R26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="S26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="T26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="U26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="V26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="W26" s="9">
-        <f t="shared" si="8"/>
+        <f t="shared" si="6"/>
         <v>50</v>
       </c>
       <c r="X26" s="15">
@@ -7545,87 +7557,87 @@
         <v>59</v>
       </c>
       <c r="C29" s="9">
-        <f t="shared" ref="C29:W29" si="9">C26+C22</f>
+        <f t="shared" ref="C29:W29" si="7">C26+C22</f>
         <v>-50.75</v>
       </c>
       <c r="D29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="E29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="F29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="G29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="H29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="I29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="J29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="K29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="L29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="M29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="N29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="O29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="P29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="Q29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="R29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="S29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="T29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="U29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="V29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="W29" s="9">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>49.25</v>
       </c>
       <c r="X29" s="15">
@@ -7640,7 +7652,7 @@
     </row>
     <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="B32" s="5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C32" s="14" t="s">
         <v>6</v>
@@ -7705,7 +7717,7 @@
     </row>
     <row r="33" spans="1:32" x14ac:dyDescent="0.25">
       <c r="B33" s="5" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="C33" s="14">
         <v>0.33329999999999999</v>
@@ -7737,476 +7749,544 @@
       <c r="V33" s="14"/>
     </row>
     <row r="34" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="B34" s="5"/>
-    </row>
-    <row r="36" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="s">
+      <c r="B34" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C34" s="46">
+        <f>$B$38*C33*-1</f>
+        <v>1314.5440181014349</v>
+      </c>
+      <c r="D34" s="46">
+        <f t="shared" ref="D34:F34" si="8">$B$38*D33*-1</f>
+        <v>1753.1197601142751</v>
+      </c>
+      <c r="E34" s="46">
+        <f t="shared" si="8"/>
+        <v>584.11031827429508</v>
+      </c>
+      <c r="F34" s="46">
+        <f t="shared" si="8"/>
+        <v>292.25236045999497</v>
+      </c>
+      <c r="W34" s="46"/>
+    </row>
+    <row r="35" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="B35" s="5" t="s">
+        <v>76</v>
+      </c>
+      <c r="C35" s="46">
+        <f>C33*$B$38*(1-$B$9)</f>
+        <v>-985.9080135760762</v>
+      </c>
+      <c r="D35" s="46">
+        <f t="shared" ref="D35:F35" si="9">D33*$B$38*(1-$B$9)</f>
+        <v>-1314.8398200857064</v>
+      </c>
+      <c r="E35" s="46">
+        <f t="shared" si="9"/>
+        <v>-438.08273870572134</v>
+      </c>
+      <c r="F35" s="46">
+        <f t="shared" si="9"/>
+        <v>-219.18927034499623</v>
+      </c>
+      <c r="W35" s="46"/>
+    </row>
+    <row r="36" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A37" s="38" t="s">
         <v>58</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B37" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="14" t="s">
+      <c r="C37" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="D36" s="14" t="s">
+      <c r="D37" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="E36" s="14" t="s">
+      <c r="E37" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="14" t="s">
+      <c r="F37" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="G36" s="14" t="s">
+      <c r="G37" s="35" t="s">
         <v>10</v>
       </c>
-      <c r="H36" s="14" t="s">
+      <c r="H37" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I36" s="14" t="s">
+      <c r="I37" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="J36" s="14" t="s">
+      <c r="J37" s="35" t="s">
         <v>13</v>
       </c>
-      <c r="K36" s="14" t="s">
+      <c r="K37" s="35" t="s">
         <v>14</v>
       </c>
-      <c r="L36" s="14" t="s">
+      <c r="L37" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="M36" s="14" t="s">
+      <c r="M37" s="35" t="s">
         <v>16</v>
       </c>
-      <c r="N36" s="14" t="s">
+      <c r="N37" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="O36" s="14" t="s">
+      <c r="O37" s="35" t="s">
         <v>18</v>
       </c>
-      <c r="P36" s="14" t="s">
+      <c r="P37" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="Q36" s="14" t="s">
+      <c r="Q37" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="R36" s="14" t="s">
+      <c r="R37" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="S36" s="14" t="s">
+      <c r="S37" s="35" t="s">
         <v>22</v>
       </c>
-      <c r="T36" s="14" t="s">
+      <c r="T37" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="U36" s="14" t="s">
+      <c r="U37" s="35" t="s">
         <v>24</v>
       </c>
-      <c r="V36" s="14" t="s">
+      <c r="V37" s="35" t="s">
         <v>25</v>
       </c>
-      <c r="W36" s="14"/>
-      <c r="X36" s="14"/>
-      <c r="Y36" s="14"/>
-      <c r="Z36" s="14"/>
-      <c r="AA36" s="14"/>
-      <c r="AB36" s="14"/>
-      <c r="AC36" s="14"/>
-      <c r="AD36" s="14"/>
-      <c r="AE36" s="14"/>
-      <c r="AF36" s="14"/>
-    </row>
-    <row r="37" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A37" s="29"/>
-      <c r="B37" s="17">
-        <f>$B$43*($C$15/$B$44)^$B$45</f>
-        <v>-1666.02</v>
-      </c>
-      <c r="C37" s="18">
-        <f>$X$29</f>
-        <v>934.25</v>
-      </c>
-      <c r="D37" s="18">
-        <f t="shared" ref="D37:U37" si="10">$X$29</f>
-        <v>934.25</v>
-      </c>
-      <c r="E37" s="18">
+      <c r="W37" s="14"/>
+      <c r="X37" s="14"/>
+      <c r="Y37" s="14"/>
+      <c r="Z37" s="14"/>
+      <c r="AA37" s="14"/>
+      <c r="AB37" s="14"/>
+      <c r="AC37" s="14"/>
+      <c r="AD37" s="14"/>
+      <c r="AE37" s="14"/>
+      <c r="AF37" s="14"/>
+    </row>
+    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A38" s="38"/>
+      <c r="B38" s="30">
+        <f>$B$44*($C$15/$B$45)^$B$46</f>
+        <v>-3944.02645695</v>
+      </c>
+      <c r="C38" s="45">
+        <f>$X$29+C35+C34</f>
+        <v>1262.8860045253587</v>
+      </c>
+      <c r="D38" s="45">
+        <f t="shared" ref="D38:F38" si="10">$X$29+D35+D34</f>
+        <v>1372.5299400285687</v>
+      </c>
+      <c r="E38" s="45">
         <f t="shared" si="10"/>
-        <v>934.25</v>
-      </c>
-      <c r="F37" s="18"/>
-      <c r="G37" s="18"/>
-      <c r="H37" s="18"/>
-      <c r="I37" s="18"/>
-      <c r="J37" s="18"/>
-      <c r="K37" s="18"/>
-      <c r="L37" s="18"/>
-      <c r="M37" s="18"/>
-      <c r="N37" s="18"/>
-      <c r="O37" s="18"/>
-      <c r="P37" s="18"/>
-      <c r="Q37" s="18"/>
-      <c r="R37" s="18"/>
-      <c r="S37" s="18"/>
-      <c r="T37" s="18"/>
-      <c r="U37" s="18"/>
-      <c r="V37" s="18"/>
-      <c r="W37" s="25"/>
-      <c r="X37" s="25"/>
-      <c r="Y37" s="25"/>
-      <c r="Z37" s="25"/>
-      <c r="AA37" s="25"/>
-      <c r="AB37" s="25"/>
-      <c r="AC37" s="25"/>
-      <c r="AD37" s="25"/>
-      <c r="AE37" s="25"/>
-      <c r="AF37" s="25"/>
-    </row>
-    <row r="38" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A38" s="5" t="s">
+        <v>1080.2775795685739</v>
+      </c>
+      <c r="F38" s="31">
+        <f t="shared" si="10"/>
+        <v>1007.3130901149988</v>
+      </c>
+      <c r="G38" s="36"/>
+      <c r="H38" s="36"/>
+      <c r="I38" s="36"/>
+      <c r="J38" s="36"/>
+      <c r="K38" s="36"/>
+      <c r="L38" s="36"/>
+      <c r="M38" s="36"/>
+      <c r="N38" s="36"/>
+      <c r="O38" s="36"/>
+      <c r="P38" s="36"/>
+      <c r="Q38" s="36"/>
+      <c r="R38" s="36"/>
+      <c r="S38" s="36"/>
+      <c r="T38" s="36"/>
+      <c r="U38" s="36"/>
+      <c r="V38" s="36"/>
+      <c r="W38" s="46"/>
+      <c r="X38" s="23"/>
+      <c r="Y38" s="23"/>
+      <c r="Z38" s="23"/>
+      <c r="AA38" s="23"/>
+      <c r="AB38" s="23"/>
+      <c r="AC38" s="23"/>
+      <c r="AD38" s="23"/>
+      <c r="AE38" s="23"/>
+      <c r="AF38" s="23"/>
+    </row>
+    <row r="39" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B38" s="22">
-        <f>NPV($B$7,C37:AF37)+$B$37</f>
-        <v>741.6328603363304</v>
-      </c>
-    </row>
-    <row r="41" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+      <c r="B39" s="32">
+        <f>NPV($B$7,C38:AF38)+$B$38</f>
+        <v>1.9394974515307695E-9</v>
+      </c>
+      <c r="C39" s="33"/>
+      <c r="D39" s="33"/>
+      <c r="E39" s="33"/>
+      <c r="F39" s="34"/>
+      <c r="G39" s="37"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="37"/>
+      <c r="N39" s="37"/>
+      <c r="O39" s="37"/>
+      <c r="P39" s="37"/>
+      <c r="Q39" s="37"/>
+      <c r="R39" s="37"/>
+      <c r="S39" s="37"/>
+      <c r="T39" s="37"/>
+      <c r="U39" s="37"/>
+      <c r="V39" s="37"/>
+      <c r="W39" s="23"/>
+    </row>
+    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="42" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A42" s="30" t="s">
+    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A43" s="39" t="s">
         <v>30</v>
       </c>
-      <c r="B42" s="31"/>
-    </row>
-    <row r="43" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A43" s="27" t="s">
+      <c r="B43" s="40"/>
+    </row>
+    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A44" s="25" t="s">
         <v>31</v>
       </c>
-      <c r="B43" s="28">
-        <v>-1666.02</v>
-      </c>
-    </row>
-    <row r="44" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A44" s="19" t="s">
+      <c r="B44" s="26">
+        <v>-3944.02645695</v>
+      </c>
+      <c r="D44" s="44"/>
+    </row>
+    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A45" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B44" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A45" s="19" t="s">
+      <c r="B45" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A46" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B45" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="46" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A46" s="19" t="s">
+      <c r="B46" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A47" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B46" s="20">
+      <c r="B47" s="19">
         <f>B2</f>
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A47" s="19" t="s">
+    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A48" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B48" s="19" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="48" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A48" s="19" t="s">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B48" s="20" t="s">
+      <c r="B49" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="19" t="s">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B49" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="19" t="s">
+      <c r="B50" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B50" s="20" t="s">
+      <c r="B51" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="19" t="s">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B51" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="19" t="s">
+      <c r="B52" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" s="18" t="s">
         <v>65</v>
       </c>
-      <c r="B52" s="20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="32" t="s">
+      <c r="B53" s="19">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="41" t="s">
         <v>28</v>
       </c>
-      <c r="B54" s="33"/>
-    </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="23" t="s">
+      <c r="B55" s="42"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B55" s="24">
+      <c r="B56" s="22">
         <v>-100</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="19" t="s">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B56" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="19" t="s">
+      <c r="B57" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B57" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A58" s="19" t="s">
+      <c r="B58" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B58" s="20">
+      <c r="B59" s="19">
         <f>B2</f>
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A59" s="19" t="s">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B59" s="20" t="s">
+      <c r="B60" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A60" s="19" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B60" s="20" t="s">
+      <c r="B61" s="19" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A61" s="19" t="s">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B61" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A62" s="19" t="s">
+      <c r="B62" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B62" s="20" t="s">
+      <c r="B63" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A63" s="19" t="s">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B63" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="34" t="s">
+      <c r="B64" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="43" t="s">
         <v>29</v>
       </c>
-      <c r="B65" s="34"/>
-    </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A66" s="23" t="s">
+      <c r="B66" s="43"/>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="B66" s="24">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A67" s="19" t="s">
+      <c r="B67" s="22">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B67" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A68" s="19" t="s">
+      <c r="B68" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B68" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A69" s="19" t="s">
+      <c r="B69" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B69" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A70" s="19" t="s">
+      <c r="B70" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B70" s="20" t="s">
+      <c r="B71" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A71" s="19" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B71" s="20" t="s">
+      <c r="B72" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A72" s="19" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B72" s="20" t="b">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A73" s="19" t="s">
+      <c r="B73" s="19" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B73" s="20" t="s">
+      <c r="B74" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A74" s="19" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A75" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B74" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A76" s="32" t="s">
+      <c r="B75" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="41" t="s">
         <v>52</v>
       </c>
-      <c r="B76" s="33"/>
-    </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A77" s="19" t="s">
+      <c r="B77" s="42"/>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A78" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="B77" s="20">
+      <c r="B78" s="19">
         <v>-50</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A78" s="19" t="s">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A79" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="B78" s="20" t="s">
+      <c r="B79" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A79" s="19" t="s">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A80" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="B79" s="20">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A80" s="19" t="s">
+      <c r="B80" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A81" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="B80" s="20">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" s="19" t="s">
+      <c r="B81" s="19">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A82" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="B81" s="20" t="s">
+      <c r="B82" s="19" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" s="19" t="s">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A83" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="B82" s="20" t="s">
+      <c r="B83" s="19" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" s="19" t="s">
+    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A84" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="B83" s="20" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" s="19" t="s">
+      <c r="B84" s="19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A85" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="B84" s="20" t="s">
+      <c r="B85" s="19" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" s="19" t="s">
+    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A86" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="B85" s="20" t="b">
+      <c r="B86" s="19" t="b">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="5">
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="A54:B54"/>
-    <mergeCell ref="A65:B65"/>
-    <mergeCell ref="A76:B76"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="A55:B55"/>
+    <mergeCell ref="A66:B66"/>
+    <mergeCell ref="A77:B77"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>